<commit_message>
Fixed misnaming issue with sequences
</commit_message>
<xml_diff>
--- a/main.xlsx
+++ b/main.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanos\Documents\Work\Columbia Research Assistant Job\PsychoPy Experiments\Cocaine_Study_Stroop_Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1962A18A-9219-4303-8E53-6C6A0A711658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F673CEE-909E-40A7-B9C5-1B73E4D4CA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{6B99EDC8-0F14-4D6E-92D5-91A7B2C74E56}"/>
+    <workbookView xWindow="13998" yWindow="0" windowWidth="8970" windowHeight="12360" xr2:uid="{6B99EDC8-0F14-4D6E-92D5-91A7B2C74E56}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,34 +38,34 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>runs/seq1_1.xlsx</t>
-  </si>
-  <si>
-    <t>runs/seq1_2_ic.xlsx</t>
-  </si>
-  <si>
-    <t>runs/seq1_3.xlsx</t>
-  </si>
-  <si>
-    <t>runs/seq2_1.xlsx</t>
-  </si>
-  <si>
-    <t>runs/seq2_2_ic.xlsx</t>
-  </si>
-  <si>
-    <t>runs/seq2_3.xlsx</t>
-  </si>
-  <si>
-    <t>runs/seq3_1.xlsx</t>
-  </si>
-  <si>
-    <t>runs/seq3_2_ic.xlsx</t>
-  </si>
-  <si>
-    <t>runs/seq3_3.xlsx</t>
-  </si>
-  <si>
     <t>blocks</t>
+  </si>
+  <si>
+    <t>runs/seq_1_1.xlsx</t>
+  </si>
+  <si>
+    <t>runs/seq_1_2_ic.xlsx</t>
+  </si>
+  <si>
+    <t>runs/seq_1_3.xlsx</t>
+  </si>
+  <si>
+    <t>runs/seq_2_1.xlsx</t>
+  </si>
+  <si>
+    <t>runs/seq_2_2_ic.xlsx</t>
+  </si>
+  <si>
+    <t>runs/seq_2_3.xlsx</t>
+  </si>
+  <si>
+    <t>runs/seq_3_1.xlsx</t>
+  </si>
+  <si>
+    <t>runs/seq_3_2_ic.xlsx</t>
+  </si>
+  <si>
+    <t>runs/seq_3_3.xlsx</t>
   </si>
 </sst>
 </file>
@@ -168,13 +168,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -515,88 +512,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2468ACA-65A2-4BF2-A83E-895F586F232F}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.26171875" customWidth="1"/>
-    <col min="2" max="2" width="24.7890625" customWidth="1"/>
-    <col min="3" max="3" width="28.20703125" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="17.7890625" customWidth="1"/>
-    <col min="6" max="6" width="16.3671875" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="3"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="7" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="7" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="7" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="7" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="7" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="7" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="8" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="9"/>
-      <c r="B11" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>